<commit_message>
Added Method in Excel Reader Class and Data Driven Test Approach without Hard Coding Data
</commit_message>
<xml_diff>
--- a/empdata.xlsx
+++ b/empdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravi_kumar62\eclipse-workspace\RestAssured_TestNG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB07AB9F-C50D-452F-BE8C-FDA8A7B0F489}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3C84BC-0FF2-418C-A973-755C9E77AB68}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F5D3FD01-3D7E-407F-9854-36E7EB071B05}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddEmpData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -426,7 +426,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>